<commit_message>
added pdf of pinyin/zhuyin
</commit_message>
<xml_diff>
--- a/ceremonies/初一（十五）禮.xlsx
+++ b/ceremonies/初一（十五）禮.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Xepht\Documents\Temple\Ceremonies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Xepht\Documents\Xepht\Scripts\Temple\phonetic guide\ceremonies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923B8B23-3712-4CF9-BEBE-EED57A06D6A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A885D099-AD11-4F29-B310-927A64E28833}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="165" windowWidth="27150" windowHeight="17385" xr2:uid="{FB00F827-A904-4C25-A418-BB86F3CE250E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{FB00F827-A904-4C25-A418-BB86F3CE250E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="120">
   <si>
     <t>row</t>
   </si>
@@ -379,9 +379,6 @@
   </si>
   <si>
     <t>zhuyin</t>
-  </si>
-  <si>
-    <t>rowZhuyin</t>
   </si>
   <si>
     <t>ㄒㄧㄢ` ㄒㄧㄤ ㄑㄩㄢˊ ㄓㄨ`</t>
@@ -746,23 +743,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F681888-619E-4FC0-B318-16F454C4E2F3}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -770,19 +771,16 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>80</v>
@@ -790,19 +788,16 @@
       <c r="D2" t="s">
         <v>81</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -810,19 +805,16 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -830,19 +822,16 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -850,19 +839,16 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -870,19 +856,16 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>3</v>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -890,19 +873,16 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>4</v>
+      <c r="B8" t="s">
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -910,19 +890,16 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9">
-        <v>4</v>
+      <c r="B9" t="s">
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -930,19 +907,16 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10">
-        <v>5</v>
+      <c r="B10" t="s">
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -950,19 +924,16 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
-      <c r="B11">
-        <v>6</v>
+      <c r="B11" t="s">
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -970,19 +941,16 @@
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12">
-        <v>6</v>
+      <c r="B12" t="s">
+        <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -990,19 +958,16 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
-      <c r="B13">
-        <v>7</v>
+      <c r="B13" t="s">
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -1010,19 +975,16 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
-      <c r="B14">
-        <v>8</v>
+      <c r="B14" t="s">
+        <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
@@ -1030,19 +992,16 @@
       <c r="D14" t="s">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
-      <c r="B15">
-        <v>8</v>
+      <c r="B15" t="s">
+        <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1050,19 +1009,16 @@
       <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
-      <c r="B16">
-        <v>9</v>
+      <c r="B16" t="s">
+        <v>7</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -1070,19 +1026,16 @@
       <c r="D16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="B17">
-        <v>9</v>
+      <c r="B17" t="s">
+        <v>10</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -1090,19 +1043,16 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
-      <c r="B18">
-        <v>10</v>
+      <c r="B18" t="s">
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -1110,18 +1060,15 @@
       <c r="D18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
@@ -1130,19 +1077,16 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
-      <c r="B20">
-        <v>11</v>
+      <c r="B20" t="s">
+        <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
@@ -1150,19 +1094,16 @@
       <c r="D20" t="s">
         <v>33</v>
       </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11</v>
       </c>
-      <c r="B21">
-        <v>11</v>
+      <c r="B21" t="s">
+        <v>10</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
@@ -1170,19 +1111,16 @@
       <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
-      <c r="B22">
-        <v>12</v>
+      <c r="B22" t="s">
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -1190,19 +1128,16 @@
       <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12</v>
       </c>
-      <c r="B23">
-        <v>12</v>
+      <c r="B23" t="s">
+        <v>10</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
@@ -1210,19 +1145,16 @@
       <c r="D23" t="s">
         <v>37</v>
       </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
-      <c r="B24">
-        <v>13</v>
+      <c r="B24" t="s">
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -1230,19 +1162,16 @@
       <c r="D24" t="s">
         <v>39</v>
       </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
-      <c r="B25">
-        <v>13</v>
+      <c r="B25" t="s">
+        <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
@@ -1250,19 +1179,16 @@
       <c r="D25" t="s">
         <v>37</v>
       </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14</v>
       </c>
-      <c r="B26">
-        <v>14</v>
+      <c r="B26" t="s">
+        <v>7</v>
       </c>
       <c r="C26" t="s">
         <v>40</v>
@@ -1270,19 +1196,16 @@
       <c r="D26" t="s">
         <v>41</v>
       </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14</v>
       </c>
-      <c r="B27">
-        <v>14</v>
+      <c r="B27" t="s">
+        <v>10</v>
       </c>
       <c r="C27" t="s">
         <v>36</v>
@@ -1290,19 +1213,16 @@
       <c r="D27" t="s">
         <v>37</v>
       </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
-      <c r="B28">
-        <v>15</v>
+      <c r="B28" t="s">
+        <v>7</v>
       </c>
       <c r="C28" t="s">
         <v>42</v>
@@ -1310,19 +1230,16 @@
       <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
-      <c r="B29">
-        <v>15</v>
+      <c r="B29" t="s">
+        <v>10</v>
       </c>
       <c r="C29" t="s">
         <v>36</v>
@@ -1330,19 +1247,16 @@
       <c r="D29" t="s">
         <v>37</v>
       </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16</v>
       </c>
-      <c r="B30">
-        <v>16</v>
+      <c r="B30" t="s">
+        <v>7</v>
       </c>
       <c r="C30" t="s">
         <v>44</v>
@@ -1350,19 +1264,16 @@
       <c r="D30" t="s">
         <v>45</v>
       </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>16</v>
       </c>
-      <c r="B31">
-        <v>16</v>
+      <c r="B31" t="s">
+        <v>10</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
@@ -1370,19 +1281,16 @@
       <c r="D31" t="s">
         <v>37</v>
       </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>17</v>
       </c>
-      <c r="B32">
-        <v>17</v>
+      <c r="B32" t="s">
+        <v>7</v>
       </c>
       <c r="C32" t="s">
         <v>46</v>
@@ -1390,19 +1298,16 @@
       <c r="D32" t="s">
         <v>47</v>
       </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>17</v>
       </c>
-      <c r="B33">
-        <v>17</v>
+      <c r="B33" t="s">
+        <v>10</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
@@ -1410,19 +1315,16 @@
       <c r="D33" t="s">
         <v>37</v>
       </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>18</v>
       </c>
-      <c r="B34">
-        <v>18</v>
+      <c r="B34" t="s">
+        <v>7</v>
       </c>
       <c r="C34" t="s">
         <v>48</v>
@@ -1430,19 +1332,16 @@
       <c r="D34" t="s">
         <v>49</v>
       </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>18</v>
       </c>
-      <c r="B35">
-        <v>18</v>
+      <c r="B35" t="s">
+        <v>10</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
@@ -1450,19 +1349,16 @@
       <c r="D35" t="s">
         <v>37</v>
       </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>19</v>
       </c>
-      <c r="B36">
-        <v>19</v>
+      <c r="B36" t="s">
+        <v>7</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -1470,19 +1366,16 @@
       <c r="D36" t="s">
         <v>51</v>
       </c>
-      <c r="E36" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>19</v>
       </c>
-      <c r="B37">
-        <v>19</v>
+      <c r="B37" t="s">
+        <v>10</v>
       </c>
       <c r="C37" t="s">
         <v>52</v>
@@ -1490,19 +1383,16 @@
       <c r="D37" t="s">
         <v>53</v>
       </c>
-      <c r="E37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20</v>
       </c>
-      <c r="B38">
-        <v>20</v>
+      <c r="B38" t="s">
+        <v>7</v>
       </c>
       <c r="C38" t="s">
         <v>54</v>
@@ -1510,19 +1400,16 @@
       <c r="D38" t="s">
         <v>55</v>
       </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20</v>
       </c>
-      <c r="B39">
-        <v>20</v>
+      <c r="B39" t="s">
+        <v>10</v>
       </c>
       <c r="C39" t="s">
         <v>52</v>
@@ -1530,19 +1417,16 @@
       <c r="D39" t="s">
         <v>53</v>
       </c>
-      <c r="E39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>21</v>
       </c>
-      <c r="B40">
-        <v>21</v>
+      <c r="B40" t="s">
+        <v>7</v>
       </c>
       <c r="C40" t="s">
         <v>56</v>
@@ -1550,19 +1434,16 @@
       <c r="D40" t="s">
         <v>57</v>
       </c>
-      <c r="E40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>21</v>
       </c>
-      <c r="B41">
-        <v>21</v>
+      <c r="B41" t="s">
+        <v>10</v>
       </c>
       <c r="C41" t="s">
         <v>52</v>
@@ -1570,19 +1451,16 @@
       <c r="D41" t="s">
         <v>53</v>
       </c>
-      <c r="E41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>22</v>
       </c>
-      <c r="B42">
-        <v>22</v>
+      <c r="B42" t="s">
+        <v>7</v>
       </c>
       <c r="C42" t="s">
         <v>58</v>
@@ -1590,19 +1468,16 @@
       <c r="D42" t="s">
         <v>59</v>
       </c>
-      <c r="E42" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>22</v>
       </c>
-      <c r="B43">
-        <v>22</v>
+      <c r="B43" t="s">
+        <v>10</v>
       </c>
       <c r="C43" t="s">
         <v>52</v>
@@ -1610,19 +1485,16 @@
       <c r="D43" t="s">
         <v>53</v>
       </c>
-      <c r="E43" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>23</v>
       </c>
-      <c r="B44">
-        <v>23</v>
+      <c r="B44" t="s">
+        <v>7</v>
       </c>
       <c r="C44" t="s">
         <v>60</v>
@@ -1630,19 +1502,16 @@
       <c r="D44" t="s">
         <v>61</v>
       </c>
-      <c r="E44" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>23</v>
       </c>
-      <c r="B45">
-        <v>23</v>
+      <c r="B45" t="s">
+        <v>10</v>
       </c>
       <c r="C45" t="s">
         <v>52</v>
@@ -1650,19 +1519,16 @@
       <c r="D45" t="s">
         <v>53</v>
       </c>
-      <c r="E45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>24</v>
       </c>
-      <c r="B46">
-        <v>24</v>
+      <c r="B46" t="s">
+        <v>7</v>
       </c>
       <c r="C46" t="s">
         <v>62</v>
@@ -1670,19 +1536,16 @@
       <c r="D46" t="s">
         <v>63</v>
       </c>
-      <c r="E46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>24</v>
       </c>
-      <c r="B47">
-        <v>24</v>
+      <c r="B47" t="s">
+        <v>10</v>
       </c>
       <c r="C47" t="s">
         <v>52</v>
@@ -1690,19 +1553,16 @@
       <c r="D47" t="s">
         <v>53</v>
       </c>
-      <c r="E47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>25</v>
       </c>
-      <c r="B48">
-        <v>25</v>
+      <c r="B48" t="s">
+        <v>17</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
@@ -1710,19 +1570,16 @@
       <c r="D48" t="s">
         <v>16</v>
       </c>
-      <c r="E48" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>26</v>
       </c>
-      <c r="B49">
-        <v>26</v>
+      <c r="B49" t="s">
+        <v>7</v>
       </c>
       <c r="C49" t="s">
         <v>64</v>
@@ -1730,19 +1587,16 @@
       <c r="D49" t="s">
         <v>65</v>
       </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>26</v>
       </c>
-      <c r="B50">
-        <v>26</v>
+      <c r="B50" t="s">
+        <v>10</v>
       </c>
       <c r="C50" t="s">
         <v>26</v>
@@ -1750,19 +1604,16 @@
       <c r="D50" t="s">
         <v>27</v>
       </c>
-      <c r="E50" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>27</v>
       </c>
-      <c r="B51">
-        <v>27</v>
+      <c r="B51" t="s">
+        <v>7</v>
       </c>
       <c r="C51" t="s">
         <v>66</v>
@@ -1770,19 +1621,16 @@
       <c r="D51" t="s">
         <v>67</v>
       </c>
-      <c r="E51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>27</v>
       </c>
-      <c r="B52">
-        <v>27</v>
+      <c r="B52" t="s">
+        <v>10</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -1790,19 +1638,16 @@
       <c r="D52" t="s">
         <v>27</v>
       </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>28</v>
       </c>
-      <c r="B53">
-        <v>28</v>
+      <c r="B53" t="s">
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>68</v>
@@ -1810,19 +1655,16 @@
       <c r="D53" t="s">
         <v>69</v>
       </c>
-      <c r="E53" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>28</v>
       </c>
-      <c r="B54">
-        <v>28</v>
+      <c r="B54" t="s">
+        <v>10</v>
       </c>
       <c r="C54" t="s">
         <v>26</v>
@@ -1830,19 +1672,16 @@
       <c r="D54" t="s">
         <v>27</v>
       </c>
-      <c r="E54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>29</v>
       </c>
-      <c r="B55">
-        <v>29</v>
+      <c r="B55" t="s">
+        <v>7</v>
       </c>
       <c r="C55" t="s">
         <v>70</v>
@@ -1850,19 +1689,16 @@
       <c r="D55" t="s">
         <v>71</v>
       </c>
-      <c r="E55" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>29</v>
       </c>
-      <c r="B56">
-        <v>29</v>
+      <c r="B56" t="s">
+        <v>10</v>
       </c>
       <c r="C56" t="s">
         <v>36</v>
@@ -1870,19 +1706,16 @@
       <c r="D56" t="s">
         <v>37</v>
       </c>
-      <c r="E56" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>30</v>
       </c>
-      <c r="B57">
-        <v>30</v>
+      <c r="B57" t="s">
+        <v>7</v>
       </c>
       <c r="C57" t="s">
         <v>72</v>
@@ -1890,19 +1723,16 @@
       <c r="D57" t="s">
         <v>73</v>
       </c>
-      <c r="E57" t="s">
-        <v>7</v>
-      </c>
-      <c r="F57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>30</v>
       </c>
-      <c r="B58">
-        <v>30</v>
+      <c r="B58" t="s">
+        <v>10</v>
       </c>
       <c r="C58" t="s">
         <v>36</v>
@@ -1910,19 +1740,16 @@
       <c r="D58" t="s">
         <v>37</v>
       </c>
-      <c r="E58" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>31</v>
       </c>
-      <c r="B59">
-        <v>31</v>
+      <c r="B59" t="s">
+        <v>7</v>
       </c>
       <c r="C59" t="s">
         <v>74</v>
@@ -1930,19 +1757,16 @@
       <c r="D59" t="s">
         <v>75</v>
       </c>
-      <c r="E59" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>31</v>
       </c>
-      <c r="B60">
-        <v>31</v>
+      <c r="B60" t="s">
+        <v>10</v>
       </c>
       <c r="C60" t="s">
         <v>36</v>
@@ -1950,19 +1774,16 @@
       <c r="D60" t="s">
         <v>37</v>
       </c>
-      <c r="E60" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>32</v>
       </c>
-      <c r="B61">
-        <v>32</v>
+      <c r="B61" t="s">
+        <v>7</v>
       </c>
       <c r="C61" t="s">
         <v>76</v>
@@ -1970,19 +1791,16 @@
       <c r="D61" t="s">
         <v>77</v>
       </c>
-      <c r="E61" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>32</v>
       </c>
-      <c r="B62">
-        <v>32</v>
+      <c r="B62" t="s">
+        <v>10</v>
       </c>
       <c r="C62" t="s">
         <v>78</v>
@@ -1990,10 +1808,7 @@
       <c r="D62" t="s">
         <v>79</v>
       </c>
-      <c r="E62" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>